<commit_message>
Test1 - KPI Sensors Lanes is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/otto.xlsx
+++ b/src/test/test_data/otto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\Otto\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F49F11-D4F5-42DA-833F-1852EBE3773B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84584661-BF88-488E-95A7-395F85A2FBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>tc_id</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>test_user_123@test.com</t>
+  </si>
+  <si>
+    <t>Camera System VT1</t>
+  </si>
+  <si>
+    <t>program</t>
   </si>
 </sst>
 </file>
@@ -600,7 +606,7 @@
   <dimension ref="A1:AE29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +695,9 @@
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -727,7 +735,9 @@
       <c r="C4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>

</xml_diff>